<commit_message>
Add ECP and BVA tests for adding a product
</commit_message>
<xml_diff>
--- a/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23916"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA93D3C1-32C2-47F4-B802-E84BDAFF979C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3AC4F226-B7F0-4D8D-A6DD-A779C4D57F5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1289,31 +1289,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1349,6 +1328,27 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1367,6 +1367,12 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1415,11 +1421,50 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1436,57 +1481,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1537,36 +1567,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2025,7 +2025,7 @@
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="2:17">
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="41" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="1"/>
@@ -2162,14 +2162,14 @@
       <c r="E1" s="72"/>
     </row>
     <row r="4" spans="2:17">
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="50"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="44"/>
     </row>
     <row r="5" spans="2:17">
       <c r="B5" s="15" t="s">
@@ -2182,101 +2182,101 @@
       <c r="G5" s="15"/>
     </row>
     <row r="7" spans="2:17">
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="G7" s="80" t="s">
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="G7" s="82" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="80"/>
-      <c r="N7" s="80"/>
-      <c r="O7" s="80"/>
-      <c r="P7" s="80"/>
-      <c r="Q7" s="80"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="82"/>
+      <c r="P7" s="82"/>
+      <c r="Q7" s="82"/>
     </row>
     <row r="8" spans="2:17">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="84" t="s">
+      <c r="G8" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="86" t="s">
+      <c r="H8" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="81" t="s">
+      <c r="I8" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="82"/>
-      <c r="K8" s="82"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="82"/>
-      <c r="N8" s="82"/>
-      <c r="O8" s="83"/>
-      <c r="P8" s="88" t="s">
+      <c r="J8" s="84"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="84"/>
+      <c r="M8" s="84"/>
+      <c r="N8" s="84"/>
+      <c r="O8" s="85"/>
+      <c r="P8" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="Q8" s="88"/>
+      <c r="Q8" s="90"/>
     </row>
     <row r="9" spans="2:17" ht="49.5" customHeight="1">
-      <c r="B9" s="41">
+      <c r="B9" s="65">
         <v>1</v>
       </c>
-      <c r="C9" s="91" t="s">
+      <c r="C9" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="43" t="s">
+      <c r="E9" s="65"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="43" t="s">
+      <c r="K9" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="44" t="s">
+      <c r="L9" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="M9" s="44" t="s">
+      <c r="M9" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="N9" s="81"/>
-      <c r="O9" s="83"/>
-      <c r="P9" s="81" t="s">
+      <c r="N9" s="83"/>
+      <c r="O9" s="85"/>
+      <c r="P9" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="Q9" s="83"/>
+      <c r="Q9" s="85"/>
     </row>
     <row r="10" spans="2:17" ht="21.75" customHeight="1">
-      <c r="B10" s="41">
+      <c r="B10" s="65">
         <v>2</v>
       </c>
-      <c r="C10" s="91"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41" t="s">
+      <c r="C10" s="75"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65" t="s">
         <v>42</v>
       </c>
       <c r="G10" s="23">
@@ -2300,24 +2300,24 @@
       <c r="M10" s="39">
         <v>10</v>
       </c>
-      <c r="N10" s="75"/>
-      <c r="O10" s="76"/>
-      <c r="P10" s="75" t="s">
+      <c r="N10" s="77"/>
+      <c r="O10" s="78"/>
+      <c r="P10" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="Q10" s="76"/>
+      <c r="Q10" s="78"/>
     </row>
     <row r="11" spans="2:17" ht="26.25" customHeight="1">
-      <c r="B11" s="41">
+      <c r="B11" s="65">
         <v>3</v>
       </c>
-      <c r="C11" s="92" t="s">
+      <c r="C11" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="41"/>
+      <c r="E11" s="65"/>
       <c r="G11" s="23">
         <v>2</v>
       </c>
@@ -2339,26 +2339,26 @@
       <c r="M11" s="39">
         <v>10</v>
       </c>
-      <c r="N11" s="75"/>
-      <c r="O11" s="76"/>
-      <c r="P11" s="75" t="s">
+      <c r="N11" s="77"/>
+      <c r="O11" s="78"/>
+      <c r="P11" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="Q11" s="76"/>
+      <c r="Q11" s="78"/>
     </row>
     <row r="12" spans="2:17" ht="26.25" customHeight="1">
-      <c r="B12" s="41">
+      <c r="B12" s="65">
         <v>4</v>
       </c>
-      <c r="C12" s="92"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41" t="s">
+      <c r="C12" s="76"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="55">
+      <c r="G12" s="48">
         <v>3</v>
       </c>
-      <c r="H12" s="54">
+      <c r="H12" s="47">
         <v>3</v>
       </c>
       <c r="I12" s="39" t="s">
@@ -2376,18 +2376,18 @@
       <c r="M12" s="39">
         <v>10</v>
       </c>
-      <c r="N12" s="75"/>
-      <c r="O12" s="76"/>
-      <c r="P12" s="75" t="s">
+      <c r="N12" s="77"/>
+      <c r="O12" s="78"/>
+      <c r="P12" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="Q12" s="76"/>
+      <c r="Q12" s="78"/>
     </row>
     <row r="13" spans="2:17" ht="31.5" customHeight="1">
-      <c r="G13" s="55">
+      <c r="G13" s="48">
         <v>4</v>
       </c>
-      <c r="H13" s="54">
+      <c r="H13" s="47">
         <v>4</v>
       </c>
       <c r="I13" s="39" t="s">
@@ -2396,7 +2396,7 @@
       <c r="J13" s="39">
         <v>5</v>
       </c>
-      <c r="K13" s="54">
+      <c r="K13" s="47">
         <v>-3</v>
       </c>
       <c r="L13" s="39">
@@ -2405,16 +2405,16 @@
       <c r="M13" s="39">
         <v>10</v>
       </c>
-      <c r="N13" s="89"/>
-      <c r="O13" s="90"/>
-      <c r="P13" s="77" t="s">
+      <c r="N13" s="91"/>
+      <c r="O13" s="92"/>
+      <c r="P13" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="Q13" s="78"/>
+      <c r="Q13" s="80"/>
     </row>
     <row r="16" spans="2:17">
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
     </row>
     <row r="17" spans="6:7">
       <c r="F17" s="3"/>
@@ -2426,11 +2426,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
     <mergeCell ref="P13:Q13"/>
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="B7:E7"/>
@@ -2445,6 +2440,11 @@
     <mergeCell ref="P9:Q9"/>
     <mergeCell ref="P10:Q10"/>
     <mergeCell ref="N13:O13"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2490,75 +2490,75 @@
       <c r="E1" s="72"/>
     </row>
     <row r="3" spans="2:18">
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="96" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="109"/>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="110"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="98"/>
     </row>
     <row r="5" spans="2:18">
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="45"/>
-      <c r="G5" s="80" t="s">
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="67"/>
+      <c r="G5" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="80"/>
-      <c r="M5" s="80"/>
-      <c r="N5" s="80"/>
-      <c r="O5" s="80"/>
-      <c r="P5" s="80"/>
-      <c r="Q5" s="80"/>
-      <c r="R5" s="80"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="82"/>
     </row>
     <row r="6" spans="2:18" ht="14.45" customHeight="1">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="65" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="G6" s="84" t="s">
+      <c r="G6" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="84" t="s">
+      <c r="H6" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="84" t="s">
+      <c r="I6" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="86" t="s">
+      <c r="J6" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="99" t="s">
+      <c r="K6" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="101"/>
-      <c r="M6" s="101"/>
-      <c r="N6" s="101"/>
-      <c r="O6" s="101"/>
-      <c r="P6" s="100"/>
-      <c r="Q6" s="99" t="s">
+      <c r="L6" s="104"/>
+      <c r="M6" s="104"/>
+      <c r="N6" s="104"/>
+      <c r="O6" s="104"/>
+      <c r="P6" s="103"/>
+      <c r="Q6" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="R6" s="100"/>
+      <c r="R6" s="103"/>
     </row>
     <row r="7" spans="2:18" ht="99.75" customHeight="1">
-      <c r="B7" s="102">
+      <c r="B7" s="93">
         <v>1</v>
       </c>
       <c r="C7" s="105" t="s">
@@ -2568,39 +2568,39 @@
         <v>59</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="85"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="43" t="s">
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="43" t="s">
+      <c r="L7" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="M7" s="43" t="s">
+      <c r="M7" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="N7" s="44" t="s">
+      <c r="N7" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="O7" s="44" t="s">
+      <c r="O7" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="81" t="s">
+      <c r="P7" s="63"/>
+      <c r="Q7" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="R7" s="83"/>
+      <c r="R7" s="85"/>
     </row>
     <row r="8" spans="2:18" ht="35.25" customHeight="1">
-      <c r="B8" s="103"/>
+      <c r="B8" s="94"/>
       <c r="C8" s="106"/>
       <c r="D8" s="2" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="G8" s="43">
+      <c r="G8" s="63">
         <v>1</v>
       </c>
       <c r="H8" s="9">
@@ -2626,15 +2626,15 @@
         <v>10</v>
       </c>
       <c r="P8" s="22"/>
-      <c r="Q8" s="111" t="s">
+      <c r="Q8" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="R8" s="112"/>
+      <c r="R8" s="100"/>
     </row>
     <row r="9" spans="2:18">
-      <c r="B9" s="103"/>
+      <c r="B9" s="94"/>
       <c r="C9" s="106"/>
-      <c r="D9" s="95" t="s">
+      <c r="D9" s="110" t="s">
         <v>64</v>
       </c>
       <c r="E9" s="3"/>
@@ -2666,17 +2666,17 @@
         <v>10</v>
       </c>
       <c r="P9" s="10"/>
-      <c r="Q9" s="77" t="s">
+      <c r="Q9" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="R9" s="78"/>
+      <c r="R9" s="80"/>
     </row>
     <row r="10" spans="2:18">
-      <c r="B10" s="103"/>
+      <c r="B10" s="94"/>
       <c r="C10" s="106"/>
-      <c r="D10" s="96"/>
+      <c r="D10" s="111"/>
       <c r="E10" s="3"/>
-      <c r="G10" s="43">
+      <c r="G10" s="63">
         <v>3</v>
       </c>
       <c r="H10" s="9">
@@ -2702,17 +2702,17 @@
         <v>10</v>
       </c>
       <c r="P10" s="22"/>
-      <c r="Q10" s="93" t="s">
+      <c r="Q10" s="108" t="s">
         <v>71</v>
       </c>
-      <c r="R10" s="94"/>
+      <c r="R10" s="109"/>
     </row>
     <row r="11" spans="2:18">
-      <c r="B11" s="103"/>
+      <c r="B11" s="94"/>
       <c r="C11" s="106"/>
-      <c r="D11" s="96"/>
+      <c r="D11" s="111"/>
       <c r="E11" s="3"/>
-      <c r="G11" s="43">
+      <c r="G11" s="63">
         <v>4</v>
       </c>
       <c r="H11" s="9">
@@ -2738,17 +2738,17 @@
         <v>10</v>
       </c>
       <c r="P11" s="22"/>
-      <c r="Q11" s="93" t="s">
+      <c r="Q11" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="R11" s="94"/>
+      <c r="R11" s="109"/>
     </row>
     <row r="12" spans="2:18">
-      <c r="B12" s="104"/>
+      <c r="B12" s="95"/>
       <c r="C12" s="107"/>
-      <c r="D12" s="97"/>
+      <c r="D12" s="112"/>
       <c r="E12" s="3"/>
-      <c r="G12" s="43">
+      <c r="G12" s="63">
         <v>5</v>
       </c>
       <c r="H12" s="9">
@@ -2774,16 +2774,16 @@
         <v>10</v>
       </c>
       <c r="P12" s="22"/>
-      <c r="Q12" s="93" t="s">
+      <c r="Q12" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="R12" s="94"/>
+      <c r="R12" s="109"/>
     </row>
     <row r="13" spans="2:18">
-      <c r="B13" s="102">
+      <c r="B13" s="93">
         <v>2</v>
       </c>
-      <c r="C13" s="102" t="s">
+      <c r="C13" s="93" t="s">
         <v>45</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -2816,14 +2816,14 @@
         <v>10</v>
       </c>
       <c r="P13" s="10"/>
-      <c r="Q13" s="77" t="s">
+      <c r="Q13" s="79" t="s">
         <v>71</v>
       </c>
-      <c r="R13" s="78"/>
+      <c r="R13" s="80"/>
     </row>
     <row r="14" spans="2:18">
-      <c r="B14" s="103"/>
-      <c r="C14" s="103"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="94"/>
       <c r="D14" s="2" t="s">
         <v>79</v>
       </c>
@@ -2837,33 +2837,40 @@
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="2:18">
-      <c r="B15" s="103"/>
-      <c r="C15" s="103"/>
-      <c r="D15" s="95" t="s">
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="110" t="s">
         <v>80</v>
       </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="2:18">
-      <c r="B16" s="103"/>
-      <c r="C16" s="103"/>
-      <c r="D16" s="96"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="111"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="103"/>
-      <c r="C17" s="103"/>
-      <c r="D17" s="96"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="111"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="104"/>
-      <c r="C18" s="104"/>
-      <c r="D18" s="97"/>
+      <c r="B18" s="95"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="112"/>
       <c r="E18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="D9:D12"/>
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C18"/>
     <mergeCell ref="G5:R5"/>
@@ -2875,15 +2882,8 @@
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="K6:P6"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="C7:C12"/>
     <mergeCell ref="Q12:R12"/>
     <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="D9:D12"/>
     <mergeCell ref="D15:D18"/>
     <mergeCell ref="Q10:R10"/>
     <mergeCell ref="Q11:R11"/>
@@ -2901,7 +2901,7 @@
   <dimension ref="B1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2928,69 +2928,69 @@
       <c r="E1" s="72"/>
     </row>
     <row r="3" spans="2:14">
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="125" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="116"/>
-      <c r="I3" s="116"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="117"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="127"/>
     </row>
     <row r="4" spans="2:14">
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="140" t="s">
+      <c r="C4" s="116" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="135" t="s">
+      <c r="D4" s="121" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="86" t="s">
+      <c r="E4" s="88" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="81" t="s">
+      <c r="F4" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="88" t="s">
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="86"/>
+      <c r="L4" s="88"/>
     </row>
     <row r="5" spans="2:14" ht="105" customHeight="1">
-      <c r="B5" s="134"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="136"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="43" t="s">
+      <c r="B5" s="120"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="44" t="s">
+      <c r="I5" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="44" t="s">
+      <c r="J5" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="52" t="s">
+      <c r="K5" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="L5" s="63" t="s">
+      <c r="L5" s="56" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2998,7 +2998,7 @@
       <c r="B6" s="16">
         <v>1</v>
       </c>
-      <c r="C6" s="132" t="s">
+      <c r="C6" s="118" t="s">
         <v>87</v>
       </c>
       <c r="D6" s="20" t="s">
@@ -3019,21 +3019,21 @@
       <c r="I6" s="39">
         <v>1</v>
       </c>
-      <c r="J6" s="62">
+      <c r="J6" s="55">
         <v>10</v>
       </c>
-      <c r="K6" s="58" t="s">
+      <c r="K6" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="59"/>
+      <c r="L6" s="52"/>
     </row>
     <row r="7" spans="2:14" ht="30">
       <c r="B7" s="7">
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="132"/>
-      <c r="D7" s="42" t="s">
+      <c r="C7" s="118"/>
+      <c r="D7" s="62" t="s">
         <v>90</v>
       </c>
       <c r="E7" s="7" t="s">
@@ -3051,21 +3051,21 @@
       <c r="I7" s="39">
         <v>1</v>
       </c>
-      <c r="J7" s="62">
+      <c r="J7" s="55">
         <v>10</v>
       </c>
-      <c r="K7" s="58" t="s">
+      <c r="K7" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="L7" s="59"/>
+      <c r="L7" s="52"/>
     </row>
     <row r="8" spans="2:14">
       <c r="B8" s="7">
         <f t="shared" ref="B8:B15" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="132"/>
-      <c r="D8" s="42" t="s">
+      <c r="C8" s="118"/>
+      <c r="D8" s="62" t="s">
         <v>91</v>
       </c>
       <c r="E8" s="7" t="s">
@@ -3083,21 +3083,21 @@
       <c r="I8" s="39">
         <v>1</v>
       </c>
-      <c r="J8" s="62">
+      <c r="J8" s="55">
         <v>10</v>
       </c>
-      <c r="K8" s="58" t="s">
+      <c r="K8" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="L8" s="59"/>
+      <c r="L8" s="52"/>
     </row>
     <row r="9" spans="2:14" ht="30">
       <c r="B9" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="132"/>
-      <c r="D9" s="42" t="s">
+      <c r="C9" s="118"/>
+      <c r="D9" s="62" t="s">
         <v>92</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -3109,27 +3109,27 @@
       <c r="G9" s="39">
         <v>5</v>
       </c>
-      <c r="H9" s="54">
+      <c r="H9" s="47">
         <v>-3</v>
       </c>
       <c r="I9" s="39">
         <v>1</v>
       </c>
-      <c r="J9" s="62">
+      <c r="J9" s="55">
         <v>10</v>
       </c>
-      <c r="K9" s="68" t="s">
+      <c r="K9" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="L9" s="61"/>
+      <c r="L9" s="54"/>
     </row>
     <row r="10" spans="2:14" ht="54" customHeight="1">
       <c r="B10" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="132"/>
-      <c r="D10" s="42" t="s">
+      <c r="C10" s="118"/>
+      <c r="D10" s="62" t="s">
         <v>89</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -3147,21 +3147,21 @@
       <c r="I10" s="22">
         <v>1</v>
       </c>
-      <c r="J10" s="67">
+      <c r="J10" s="60">
         <v>10</v>
       </c>
-      <c r="K10" s="66" t="s">
+      <c r="K10" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="L10" s="64"/>
+      <c r="L10" s="57"/>
     </row>
     <row r="11" spans="2:14" ht="30">
       <c r="B11" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="132"/>
-      <c r="D11" s="42" t="s">
+      <c r="C11" s="118"/>
+      <c r="D11" s="62" t="s">
         <v>89</v>
       </c>
       <c r="E11" s="7" t="s">
@@ -3179,21 +3179,21 @@
       <c r="I11" s="22">
         <v>1</v>
       </c>
-      <c r="J11" s="67">
+      <c r="J11" s="60">
         <v>10</v>
       </c>
-      <c r="K11" s="60" t="s">
+      <c r="K11" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="L11" s="57"/>
+      <c r="L11" s="50"/>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="132"/>
-      <c r="D12" s="42" t="s">
+      <c r="C12" s="118"/>
+      <c r="D12" s="62" t="s">
         <v>89</v>
       </c>
       <c r="E12" s="7" t="s">
@@ -3211,21 +3211,21 @@
       <c r="I12" s="22">
         <v>1</v>
       </c>
-      <c r="J12" s="67">
+      <c r="J12" s="60">
         <v>10</v>
       </c>
-      <c r="K12" s="66" t="s">
+      <c r="K12" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="L12" s="65"/>
+      <c r="L12" s="58"/>
     </row>
     <row r="13" spans="2:14" ht="30">
       <c r="B13" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C13" s="132"/>
-      <c r="D13" s="46" t="s">
+      <c r="C13" s="118"/>
+      <c r="D13" s="68" t="s">
         <v>89</v>
       </c>
       <c r="E13" s="17" t="s">
@@ -3243,24 +3243,24 @@
       <c r="I13" s="22">
         <v>1</v>
       </c>
-      <c r="J13" s="67">
+      <c r="J13" s="60">
         <v>10</v>
       </c>
-      <c r="K13" s="66" t="s">
+      <c r="K13" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="L13" s="65"/>
+      <c r="L13" s="58"/>
     </row>
     <row r="14" spans="2:14" ht="30">
       <c r="B14" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C14" s="132"/>
-      <c r="D14" s="46" t="s">
+      <c r="C14" s="118"/>
+      <c r="D14" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="56" t="s">
+      <c r="E14" s="49" t="s">
         <v>75</v>
       </c>
       <c r="F14" s="21" t="s">
@@ -3275,20 +3275,20 @@
       <c r="I14" s="22">
         <v>1</v>
       </c>
-      <c r="J14" s="67">
+      <c r="J14" s="60">
         <v>10</v>
       </c>
-      <c r="K14" s="66" t="s">
+      <c r="K14" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="L14" s="65"/>
+      <c r="L14" s="58"/>
     </row>
     <row r="15" spans="2:14">
       <c r="B15" s="7">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C15" s="133"/>
+      <c r="C15" s="119"/>
       <c r="D15" s="40" t="s">
         <v>89</v>
       </c>
@@ -3307,13 +3307,13 @@
       <c r="I15" s="22">
         <v>1</v>
       </c>
-      <c r="J15" s="67">
+      <c r="J15" s="60">
         <v>10</v>
       </c>
-      <c r="K15" s="60" t="s">
+      <c r="K15" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="L15" s="57"/>
+      <c r="L15" s="50"/>
     </row>
     <row r="16" spans="2:14">
       <c r="B16" s="18"/>
@@ -3342,8 +3342,8 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="131"/>
-      <c r="L17" s="131"/>
+      <c r="K17" s="141"/>
+      <c r="L17" s="141"/>
       <c r="M17" s="4"/>
     </row>
     <row r="18" spans="2:16" ht="15.75" thickBot="1">
@@ -3351,34 +3351,34 @@
       <c r="M18" s="4"/>
     </row>
     <row r="19" spans="2:16" ht="15.75" thickTop="1">
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="132" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="123"/>
-      <c r="E19" s="123"/>
-      <c r="F19" s="124"/>
+      <c r="D19" s="133"/>
+      <c r="E19" s="133"/>
+      <c r="F19" s="134"/>
       <c r="G19" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="H19" s="122" t="s">
+      <c r="H19" s="132" t="s">
         <v>96</v>
       </c>
-      <c r="I19" s="125"/>
-      <c r="J19" s="123"/>
-      <c r="K19" s="123"/>
-      <c r="L19" s="124"/>
-      <c r="M19" s="122" t="s">
+      <c r="I19" s="135"/>
+      <c r="J19" s="133"/>
+      <c r="K19" s="133"/>
+      <c r="L19" s="134"/>
+      <c r="M19" s="132" t="s">
         <v>97</v>
       </c>
-      <c r="N19" s="125"/>
-      <c r="O19" s="123"/>
-      <c r="P19" s="124"/>
+      <c r="N19" s="135"/>
+      <c r="O19" s="133"/>
+      <c r="P19" s="134"/>
     </row>
     <row r="20" spans="2:16" ht="14.45" customHeight="1">
-      <c r="B20" s="137" t="s">
+      <c r="B20" s="123" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="138" t="s">
+      <c r="C20" s="124" t="s">
         <v>98</v>
       </c>
       <c r="D20" s="113" t="s">
@@ -3390,13 +3390,13 @@
       <c r="F20" s="114" t="s">
         <v>101</v>
       </c>
-      <c r="G20" s="130" t="s">
+      <c r="G20" s="140" t="s">
         <v>102</v>
       </c>
-      <c r="H20" s="126" t="s">
+      <c r="H20" s="136" t="s">
         <v>103</v>
       </c>
-      <c r="I20" s="127"/>
+      <c r="I20" s="137"/>
       <c r="J20" s="113" t="s">
         <v>98</v>
       </c>
@@ -3406,7 +3406,7 @@
       <c r="L20" s="114" t="s">
         <v>100</v>
       </c>
-      <c r="M20" s="120" t="s">
+      <c r="M20" s="130" t="s">
         <v>103</v>
       </c>
       <c r="N20" s="113" t="s">
@@ -3420,18 +3420,18 @@
       </c>
     </row>
     <row r="21" spans="2:16">
-      <c r="B21" s="137"/>
-      <c r="C21" s="138"/>
+      <c r="B21" s="123"/>
+      <c r="C21" s="124"/>
       <c r="D21" s="113"/>
       <c r="E21" s="113"/>
       <c r="F21" s="114"/>
-      <c r="G21" s="130"/>
-      <c r="H21" s="128"/>
-      <c r="I21" s="129"/>
+      <c r="G21" s="140"/>
+      <c r="H21" s="138"/>
+      <c r="I21" s="139"/>
       <c r="J21" s="113"/>
       <c r="K21" s="113"/>
       <c r="L21" s="114"/>
-      <c r="M21" s="121"/>
+      <c r="M21" s="131"/>
       <c r="N21" s="113"/>
       <c r="O21" s="113"/>
       <c r="P21" s="114"/>
@@ -3442,10 +3442,10 @@
       </c>
       <c r="C22" s="26">
         <f>SUM(D22:E22)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D22" s="28">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E22" s="28">
         <v>0</v>
@@ -3456,10 +3456,10 @@
       <c r="G22" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="H22" s="118" t="s">
+      <c r="H22" s="128" t="s">
         <v>104</v>
       </c>
-      <c r="I22" s="119"/>
+      <c r="I22" s="129"/>
       <c r="J22" s="2">
         <f>SUM(K22:L22)</f>
         <v>0</v>
@@ -3489,18 +3489,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C6:C15"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
     <mergeCell ref="O20:O21"/>
     <mergeCell ref="P20:P21"/>
     <mergeCell ref="F4:J4"/>
@@ -3517,6 +3505,18 @@
     <mergeCell ref="L20:L21"/>
     <mergeCell ref="K17:L17"/>
     <mergeCell ref="M19:P19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C15"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3525,15 +3525,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C96AF2D6F4A0484C94105BA9987FC7D9" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e1fbd8a4f3ed8c013dc022fb81f67eb3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c85a2994-b133-49e3-84cc-c79bd127aa10" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5573eba965dfe255846203d3c9967e9" ns2:_="">
     <xsd:import namespace="c85a2994-b133-49e3-84cc-c79bd127aa10"/>
@@ -3691,10 +3682,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{666863EB-81C6-4452-8CD0-2C6312330A9F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B813259-2D8C-446D-8B36-A2B645F5990D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B813259-2D8C-446D-8B36-A2B645F5990D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{666863EB-81C6-4452-8CD0-2C6312330A9F}"/>
 </file>
</xml_diff>